<commit_message>
Game snake following evaluations done: only_semantic_smells, only_syntactic_smells, random_01, random_02. Hotfixes for other evaluations are done. Sync with the evaluations in drive later.
</commit_message>
<xml_diff>
--- a/evaluations/GPT/2025-03-31_103806/snake/all_smells_01/evaluation.xlsx
+++ b/evaluations/GPT/2025-03-31_103806/snake/all_smells_01/evaluation.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="22">
   <si>
     <t>Requirement ID</t>
   </si>
@@ -62,6 +62,9 @@
   </si>
   <si>
     <t>1.5.3</t>
+  </si>
+  <si>
+    <t>1.3.1, 1.5.3</t>
   </si>
   <si>
     <t>2.5.1, 2.5.3</t>
@@ -602,13 +605,13 @@
         <v>0.0</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="E13" s="1">
         <v>0.0</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="G13" s="3"/>
       <c r="H13" s="3"/>
@@ -631,7 +634,7 @@
         <v>0.0</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="G14" s="3"/>
       <c r="H14" s="3"/>
@@ -648,13 +651,13 @@
         <v>0.0</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E15" s="1">
         <v>0.0</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="G15" s="3"/>
       <c r="H15" s="3"/>
@@ -662,7 +665,7 @@
     </row>
     <row r="16">
       <c r="A16" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B16" s="1"/>
       <c r="C16" s="3">

</xml_diff>

<commit_message>
Game snake evaluation CSV files added. Evaluation analysis skeleton code added.
</commit_message>
<xml_diff>
--- a/evaluations/GPT/2025-03-31_103806/snake/all_smells_01/evaluation.xlsx
+++ b/evaluations/GPT/2025-03-31_103806/snake/all_smells_01/evaluation.xlsx
@@ -795,10 +795,7 @@
     <row r="27">
       <c r="C27" s="3"/>
       <c r="D27" s="3"/>
-      <c r="E27" s="3">
-        <f>SUM(E2:E26)</f>
-        <v>16</v>
-      </c>
+      <c r="E27" s="3"/>
       <c r="F27" s="3"/>
     </row>
   </sheetData>

</xml_diff>